<commit_message>
updated csv and feature files
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="141">
   <si>
     <t>Add</t>
   </si>
@@ -1139,26 +1139,47 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="P7" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="15">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="P8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>21</v>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="15">

</xml_diff>

<commit_message>
Added multiple Benefit plan, Added multiple  -Payment Appendix to Include, new amendments steps added for MGA, Regular Appendix method update, Provider details method update, added new class BenefitPlanDescriptionsProvision, updated I click Make Correction
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="143">
   <si>
     <t>Add</t>
   </si>
@@ -446,6 +446,12 @@
   </si>
   <si>
     <t>2649796</t>
+  </si>
+  <si>
+    <t>352047838</t>
+  </si>
+  <si>
+    <t>1739454</t>
   </si>
 </sst>
 </file>
@@ -1182,15 +1188,30 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="P9" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>22</v>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="15">

</xml_diff>

<commit_message>
Updated Cen and West TC
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="145">
   <si>
     <t>Add</t>
   </si>
@@ -452,6 +452,12 @@
   </si>
   <si>
     <t>1739454</t>
+  </si>
+  <si>
+    <t>351752500</t>
+  </si>
+  <si>
+    <t>710493</t>
   </si>
 </sst>
 </file>
@@ -1243,15 +1249,36 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="P11" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>24</v>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" t="s">
+        <v>129</v>
+      </c>
+      <c r="H11" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" t="s">
+        <v>129</v>
+      </c>
+      <c r="J11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="15">

</xml_diff>

<commit_message>
Specialist to PCP  added
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="147">
   <si>
     <t>Add</t>
   </si>
@@ -1401,28 +1401,95 @@
         <v>129</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="P15" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15">
-      <c r="A16">
-        <f t="shared" si="1" ref="A16:A56">A15+1</f>
-        <v>15</v>
-      </c>
-      <c r="P16" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>29</v>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" t="s">
+        <v>129</v>
+      </c>
+      <c r="F15" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" t="s">
+        <v>129</v>
+      </c>
+      <c r="I15" t="s">
+        <v>129</v>
+      </c>
+      <c r="J15" t="s">
+        <v>129</v>
+      </c>
+      <c r="K15" t="s">
+        <v>129</v>
+      </c>
+      <c r="L15" t="s">
+        <v>129</v>
+      </c>
+      <c r="M15" t="s">
+        <v>129</v>
+      </c>
+      <c r="N15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" t="s">
+        <v>129</v>
+      </c>
+      <c r="G16" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" t="s">
+        <v>129</v>
+      </c>
+      <c r="I16" t="s">
+        <v>129</v>
+      </c>
+      <c r="J16" t="s">
+        <v>129</v>
+      </c>
+      <c r="K16" t="s">
+        <v>129</v>
+      </c>
+      <c r="L16" t="s">
+        <v>129</v>
+      </c>
+      <c r="M16" t="s">
+        <v>129</v>
+      </c>
+      <c r="N16" t="s">
+        <v>129</v>
+      </c>
+      <c r="O16" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="15">

</xml_diff>

<commit_message>
Updated Upload Download Functionality
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="129">
   <si>
     <t>Add</t>
   </si>
@@ -399,6 +399,18 @@
   </si>
   <si>
     <t>1071153</t>
+  </si>
+  <si>
+    <t>today</t>
+  </si>
+  <si>
+    <t>Excluded from Exchange//Excluded from ERWrap</t>
+  </si>
+  <si>
+    <t>R00</t>
+  </si>
+  <si>
+    <t>January 07, 2020</t>
   </si>
 </sst>
 </file>
@@ -1396,88 +1408,335 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" t="s">
+        <v>124</v>
+      </c>
+      <c r="J18" t="s">
+        <v>107</v>
+      </c>
+      <c r="K18" t="s">
+        <v>107</v>
+      </c>
+      <c r="L18" t="s">
+        <v>123</v>
+      </c>
+      <c r="M18" t="s">
+        <v>107</v>
+      </c>
+      <c r="N18" t="s">
+        <v>125</v>
+      </c>
+      <c r="O18" t="s">
+        <v>107</v>
       </c>
       <c r="P18" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" t="s">
+        <v>107</v>
+      </c>
+      <c r="G19" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" t="s">
+        <v>126</v>
+      </c>
+      <c r="I19" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" t="s">
+        <v>107</v>
+      </c>
+      <c r="K19" t="s">
+        <v>107</v>
+      </c>
+      <c r="L19" t="s">
+        <v>123</v>
+      </c>
+      <c r="M19" t="s">
+        <v>107</v>
+      </c>
+      <c r="N19" t="s">
+        <v>125</v>
+      </c>
+      <c r="O19" t="s">
+        <v>107</v>
       </c>
       <c r="P19" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="P20" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="P21" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="P22" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="P23" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="P24" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>26</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D20" t="s">
+        <v>107</v>
+      </c>
+      <c r="E20" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" t="s">
+        <v>107</v>
+      </c>
+      <c r="H20" t="s">
+        <v>107</v>
+      </c>
+      <c r="I20" t="s">
+        <v>107</v>
+      </c>
+      <c r="J20" t="s">
+        <v>107</v>
+      </c>
+      <c r="K20" t="s">
+        <v>107</v>
+      </c>
+      <c r="L20" t="s">
+        <v>125</v>
+      </c>
+      <c r="M20" t="s">
+        <v>127</v>
+      </c>
+      <c r="N20" t="s">
+        <v>125</v>
+      </c>
+      <c r="O20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" t="s">
+        <v>107</v>
+      </c>
+      <c r="E21" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" t="s">
+        <v>107</v>
+      </c>
+      <c r="G21" t="s">
+        <v>107</v>
+      </c>
+      <c r="H21" t="s">
+        <v>107</v>
+      </c>
+      <c r="I21" t="s">
+        <v>107</v>
+      </c>
+      <c r="J21" t="s">
+        <v>107</v>
+      </c>
+      <c r="K21" t="s">
+        <v>107</v>
+      </c>
+      <c r="L21" t="s">
+        <v>125</v>
+      </c>
+      <c r="M21" t="s">
+        <v>127</v>
+      </c>
+      <c r="N21" t="s">
+        <v>125</v>
+      </c>
+      <c r="O21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G22" t="s">
+        <v>107</v>
+      </c>
+      <c r="H22" t="s">
+        <v>107</v>
+      </c>
+      <c r="I22" t="s">
+        <v>107</v>
+      </c>
+      <c r="J22" t="s">
+        <v>107</v>
+      </c>
+      <c r="K22" t="s">
+        <v>107</v>
+      </c>
+      <c r="L22" t="s">
+        <v>128</v>
+      </c>
+      <c r="M22" t="s">
+        <v>127</v>
+      </c>
+      <c r="N22" t="s">
+        <v>128</v>
+      </c>
+      <c r="O22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" t="s">
+        <v>107</v>
+      </c>
+      <c r="H23" t="s">
+        <v>107</v>
+      </c>
+      <c r="I23" t="s">
+        <v>107</v>
+      </c>
+      <c r="J23" t="s">
+        <v>107</v>
+      </c>
+      <c r="K23" t="s">
+        <v>107</v>
+      </c>
+      <c r="L23"/>
+      <c r="M23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23"/>
+      <c r="O23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>123</v>
+      </c>
+      <c r="C24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" t="s">
+        <v>107</v>
+      </c>
+      <c r="G24" t="s">
+        <v>107</v>
+      </c>
+      <c r="H24" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" t="s">
+        <v>107</v>
+      </c>
+      <c r="J24" t="s">
+        <v>107</v>
+      </c>
+      <c r="K24" t="s">
+        <v>107</v>
+      </c>
+      <c r="L24" t="s">
+        <v>128</v>
+      </c>
+      <c r="M24" t="s">
+        <v>15</v>
+      </c>
+      <c r="N24" t="s">
+        <v>128</v>
+      </c>
+      <c r="O24" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
W4 test cases added in smga
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="134">
   <si>
     <t>Add</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t>January 24, 2020</t>
+  </si>
+  <si>
+    <t>January 28, 2020</t>
   </si>
 </sst>
 </file>
@@ -1845,16 +1848,51 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="P27" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>29</v>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" t="s">
+        <v>107</v>
+      </c>
+      <c r="G27" t="s">
+        <v>107</v>
+      </c>
+      <c r="H27" t="s">
+        <v>107</v>
+      </c>
+      <c r="I27" t="s">
+        <v>107</v>
+      </c>
+      <c r="J27" t="s">
+        <v>107</v>
+      </c>
+      <c r="K27" t="s">
+        <v>107</v>
+      </c>
+      <c r="L27" t="s">
+        <v>133</v>
+      </c>
+      <c r="M27" t="s">
+        <v>15</v>
+      </c>
+      <c r="N27" t="s">
+        <v>107</v>
+      </c>
+      <c r="O27" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Wave 4 Amendments KS1
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="135">
   <si>
     <t>Add</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>January 28, 2020</t>
+  </si>
+  <si>
+    <t>February 04, 2020</t>
   </si>
 </sst>
 </file>
@@ -1895,16 +1898,51 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="P28" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>30</v>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" t="s">
+        <v>107</v>
+      </c>
+      <c r="J28" t="s">
+        <v>107</v>
+      </c>
+      <c r="K28" t="s">
+        <v>107</v>
+      </c>
+      <c r="L28" t="s">
+        <v>134</v>
+      </c>
+      <c r="M28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" t="s">
+        <v>107</v>
+      </c>
+      <c r="O28" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Wave 4 Amendment Alabama
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="138">
   <si>
     <t>Add</t>
   </si>
@@ -426,6 +426,18 @@
   </si>
   <si>
     <t>January 28, 2020</t>
+  </si>
+  <si>
+    <t>275022892</t>
+  </si>
+  <si>
+    <t>3352838</t>
+  </si>
+  <si>
+    <t>February 04, 2020</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
@@ -1895,16 +1907,51 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="P28" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>30</v>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G28" t="s">
+        <v>107</v>
+      </c>
+      <c r="H28" t="s">
+        <v>107</v>
+      </c>
+      <c r="I28" t="s">
+        <v>107</v>
+      </c>
+      <c r="J28" t="s">
+        <v>107</v>
+      </c>
+      <c r="K28" t="s">
+        <v>107</v>
+      </c>
+      <c r="L28" t="s">
+        <v>136</v>
+      </c>
+      <c r="M28" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" t="s">
+        <v>136</v>
+      </c>
+      <c r="O28" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Add Payment Appendix Functionality in Amendments
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="113">
   <si>
     <t>Add</t>
   </si>
@@ -354,6 +354,15 @@
   </si>
   <si>
     <t>5</t>
+  </si>
+  <si>
+    <t>830392338</t>
+  </si>
+  <si>
+    <t>2420240</t>
+  </si>
+  <si>
+    <t>February 20, 2020</t>
   </si>
 </sst>
 </file>
@@ -361,10 +370,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -730,7 +739,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -749,20 +758,20 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.81640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.81640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12.54296875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.81640625" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="9" width="14.26953125" style="7" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.26953125" style="7" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="20.54296875" style="7" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="21.54296875" style="11" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="30.7265625" style="2" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.7265625" style="12" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="28.54296875" style="2" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="35.7265625" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="81.26953125" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="11.26953125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="16.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="14.81640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="12.54296875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="21.81640625" collapsed="true"/>
+    <col min="6" max="9" customWidth="true" style="7" width="14.26953125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="7" width="17.26953125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="7" width="20.54296875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" style="11" width="21.54296875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="2" width="30.7265625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="12" width="22.7265625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="2" width="28.54296875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" hidden="true" width="35.7265625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" hidden="true" width="81.26953125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="3" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1870,26 +1879,98 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="P29" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="P30" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>18</v>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>110</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" t="s">
+        <v>79</v>
+      </c>
+      <c r="H29" t="s">
+        <v>79</v>
+      </c>
+      <c r="I29" t="s">
+        <v>79</v>
+      </c>
+      <c r="J29" t="s">
+        <v>79</v>
+      </c>
+      <c r="K29" t="s">
+        <v>79</v>
+      </c>
+      <c r="L29" t="s">
+        <v>112</v>
+      </c>
+      <c r="M29" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" t="s">
+        <v>79</v>
+      </c>
+      <c r="O29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" t="s">
+        <v>79</v>
+      </c>
+      <c r="G30" t="s">
+        <v>79</v>
+      </c>
+      <c r="H30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I30" t="s">
+        <v>79</v>
+      </c>
+      <c r="J30" t="s">
+        <v>79</v>
+      </c>
+      <c r="K30" t="s">
+        <v>79</v>
+      </c>
+      <c r="L30" t="s">
+        <v>112</v>
+      </c>
+      <c r="M30" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" t="s">
+        <v>79</v>
+      </c>
+      <c r="O30" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.35">
@@ -4879,9 +4960,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.54296875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.1796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="29.54296875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Minor changes in contract number file and 1 test case
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="114">
   <si>
     <t>Add</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>February 20, 2020</t>
+  </si>
+  <si>
+    <t>February 24, 2020</t>
   </si>
 </sst>
 </file>
@@ -1973,26 +1976,98 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="P31" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="P32" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>20</v>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>110</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" t="s">
+        <v>79</v>
+      </c>
+      <c r="F31" t="s">
+        <v>79</v>
+      </c>
+      <c r="G31" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" t="s">
+        <v>79</v>
+      </c>
+      <c r="J31" t="s">
+        <v>79</v>
+      </c>
+      <c r="K31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L31" t="s">
+        <v>113</v>
+      </c>
+      <c r="M31" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" t="s">
+        <v>79</v>
+      </c>
+      <c r="O31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+      <c r="E32" t="s">
+        <v>79</v>
+      </c>
+      <c r="F32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" t="s">
+        <v>79</v>
+      </c>
+      <c r="H32" t="s">
+        <v>79</v>
+      </c>
+      <c r="I32" t="s">
+        <v>79</v>
+      </c>
+      <c r="J32" t="s">
+        <v>79</v>
+      </c>
+      <c r="K32" t="s">
+        <v>79</v>
+      </c>
+      <c r="L32" t="s">
+        <v>113</v>
+      </c>
+      <c r="M32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N32" t="s">
+        <v>79</v>
+      </c>
+      <c r="O32" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fixed Amendment for SMGA NE Wave 5
</commit_message>
<xml_diff>
--- a/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
+++ b/src/test/resources/features/rcbridge/ProviderRoster/Provider-Roster-74788257-Tue Nov 19 2019 04_52_18 GMT-0600 (CST).xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="117">
   <si>
     <t>Add</t>
   </si>
@@ -366,6 +366,15 @@
   </si>
   <si>
     <t>February 24, 2020</t>
+  </si>
+  <si>
+    <t>260826968</t>
+  </si>
+  <si>
+    <t>2903508</t>
+  </si>
+  <si>
+    <t>February 26, 2020</t>
   </si>
 </sst>
 </file>
@@ -2070,37 +2079,145 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="P33" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="P34" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="P35" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>23</v>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>114</v>
+      </c>
+      <c r="C33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" t="s">
+        <v>79</v>
+      </c>
+      <c r="E33" t="s">
+        <v>79</v>
+      </c>
+      <c r="F33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" t="s">
+        <v>79</v>
+      </c>
+      <c r="I33" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" t="s">
+        <v>79</v>
+      </c>
+      <c r="K33" t="s">
+        <v>79</v>
+      </c>
+      <c r="L33" t="s">
+        <v>116</v>
+      </c>
+      <c r="M33" t="s">
+        <v>15</v>
+      </c>
+      <c r="N33" t="s">
+        <v>116</v>
+      </c>
+      <c r="O33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" t="s">
+        <v>79</v>
+      </c>
+      <c r="H34" t="s">
+        <v>79</v>
+      </c>
+      <c r="I34" t="s">
+        <v>79</v>
+      </c>
+      <c r="J34" t="s">
+        <v>79</v>
+      </c>
+      <c r="K34" t="s">
+        <v>79</v>
+      </c>
+      <c r="L34" t="s">
+        <v>116</v>
+      </c>
+      <c r="M34" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" t="s">
+        <v>116</v>
+      </c>
+      <c r="O34" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>114</v>
+      </c>
+      <c r="C35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" t="s">
+        <v>79</v>
+      </c>
+      <c r="H35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I35" t="s">
+        <v>79</v>
+      </c>
+      <c r="J35" t="s">
+        <v>79</v>
+      </c>
+      <c r="K35" t="s">
+        <v>79</v>
+      </c>
+      <c r="L35" t="s">
+        <v>116</v>
+      </c>
+      <c r="M35" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" t="s">
+        <v>116</v>
+      </c>
+      <c r="O35" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>